<commit_message>
Solución importe de productos
</commit_message>
<xml_diff>
--- a/public/formats/items.xlsx
+++ b/public/formats/items.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brayan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\test_fact\public\formats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5034239-7C81-46D9-B4F6-8C52728BE3C7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1ACC8462-8AD9-4C4D-8C6A-33FC1AA1C04F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,9 +54,6 @@
     <t>Codigo Tipo de Afectación del Igv Compra</t>
   </si>
   <si>
-    <t>Stock</t>
-  </si>
-  <si>
     <t>Stock Mínimo</t>
   </si>
   <si>
@@ -73,6 +70,9 @@
   </si>
   <si>
     <t>P00X</t>
+  </si>
+  <si>
+    <t>Stock por almacén (separados por ; )</t>
   </si>
 </sst>
 </file>
@@ -392,8 +392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,7 +407,7 @@
     <col min="7" max="7" width="36.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -440,24 +440,24 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>20202020</v>
       </c>
       <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
         <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
       </c>
       <c r="F2">
         <v>120.25</v>
@@ -480,19 +480,19 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
       </c>
       <c r="C3">
         <v>51121703</v>
       </c>
       <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
         <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
       </c>
       <c r="F3">
         <v>150</v>

</xml_diff>